<commit_message>
1.增加 LargeWave 和 Duplicate 的特效
</commit_message>
<xml_diff>
--- a/_DESIGN_.xlsx
+++ b/_DESIGN_.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="20520" windowHeight="3930" activeTab="6"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="20520" windowHeight="3930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="游戏常数" sheetId="2" r:id="rId1"/>
@@ -2204,6 +2204,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2211,9 +2214,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2463,11 +2463,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="100104448"/>
-        <c:axId val="100114432"/>
+        <c:axId val="98777728"/>
+        <c:axId val="98804096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="100104448"/>
+        <c:axId val="98777728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2477,12 +2477,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100114432"/>
+        <c:crossAx val="98804096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100114432"/>
+        <c:axId val="98804096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2511,7 +2511,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100104448"/>
+        <c:crossAx val="98777728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7122,8 +7122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X49"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -9276,16 +9276,16 @@
         <v>29</v>
       </c>
       <c r="C31" s="77">
-        <v>88.23</v>
+        <v>48.23</v>
       </c>
       <c r="D31" s="77">
-        <v>210.08</v>
+        <v>160.08000000000001</v>
       </c>
       <c r="E31" s="70">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F31" s="70">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="G31" s="71">
         <v>79.5</v>
@@ -9295,11 +9295,11 @@
       </c>
       <c r="I31">
         <f t="shared" si="54"/>
-        <v>221.96226415094338</v>
+        <v>120.11999999999999</v>
       </c>
       <c r="J31" s="29">
         <f t="shared" si="55"/>
-        <v>4045.9851851851859</v>
+        <v>3003.9703703703703</v>
       </c>
       <c r="K31" s="31">
         <v>10</v>
@@ -9315,19 +9315,19 @@
       </c>
       <c r="O31" s="29">
         <f t="shared" si="42"/>
-        <v>2219.6226415094338</v>
+        <v>1201.1999999999998</v>
       </c>
       <c r="P31" s="29">
         <f t="shared" si="43"/>
-        <v>40459.851851851854</v>
+        <v>30039.703703703708</v>
       </c>
       <c r="Q31" s="30">
         <f t="shared" si="44"/>
-        <v>1.3810495296384451</v>
+        <v>2.319095998341282</v>
       </c>
       <c r="R31" s="30">
         <f t="shared" si="45"/>
-        <v>0.95</v>
+        <v>0.91919191919191912</v>
       </c>
       <c r="S31" s="30">
         <f t="shared" si="46"/>
@@ -9335,7 +9335,7 @@
       </c>
       <c r="T31" s="30">
         <f t="shared" si="47"/>
-        <v>17.228256954676542</v>
+        <v>24.008078341411682</v>
       </c>
       <c r="X31" s="73"/>
     </row>
@@ -14538,13 +14538,13 @@
       <c r="H3" s="13"/>
     </row>
     <row r="4" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="79">
+      <c r="B4" s="80">
         <v>0</v>
       </c>
-      <c r="C4" s="79" t="s">
+      <c r="C4" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="79" t="s">
+      <c r="D4" s="80" t="s">
         <v>50</v>
       </c>
       <c r="E4" s="15" t="s">
@@ -14572,9 +14572,9 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
+      <c r="B5" s="81"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
       <c r="E5" s="15" t="s">
         <v>1</v>
       </c>
@@ -14600,9 +14600,9 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B6" s="81"/>
-      <c r="C6" s="81"/>
-      <c r="D6" s="81"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
       <c r="E6" s="19" t="s">
         <v>2</v>
       </c>
@@ -14638,13 +14638,13 @@
       <c r="L7" s="24"/>
     </row>
     <row r="8" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="79">
+      <c r="B8" s="80">
         <v>1</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="C8" s="80" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="79" t="s">
+      <c r="D8" s="80" t="s">
         <v>52</v>
       </c>
       <c r="E8" s="21" t="s">
@@ -14672,9 +14672,9 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B9" s="80"/>
-      <c r="C9" s="80"/>
-      <c r="D9" s="80"/>
+      <c r="B9" s="81"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
       <c r="E9" s="15" t="s">
         <v>1</v>
       </c>
@@ -14700,9 +14700,9 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B10" s="80"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="80"/>
+      <c r="B10" s="81"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="81"/>
       <c r="E10" s="15" t="s">
         <v>2</v>
       </c>
@@ -14728,9 +14728,9 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B11" s="81"/>
-      <c r="C11" s="81"/>
-      <c r="D11" s="81"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="82"/>
       <c r="E11" s="19" t="s">
         <v>43</v>
       </c>
@@ -14760,13 +14760,13 @@
       <c r="K12" s="25"/>
     </row>
     <row r="13" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="79">
+      <c r="B13" s="80">
         <v>2</v>
       </c>
-      <c r="C13" s="79" t="s">
+      <c r="C13" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="79" t="s">
+      <c r="D13" s="80" t="s">
         <v>53</v>
       </c>
       <c r="E13" s="21" t="s">
@@ -14794,9 +14794,9 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
+      <c r="B14" s="81"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="81"/>
       <c r="E14" s="15" t="s">
         <v>1</v>
       </c>
@@ -14822,9 +14822,9 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B15" s="80"/>
-      <c r="C15" s="80"/>
-      <c r="D15" s="80"/>
+      <c r="B15" s="81"/>
+      <c r="C15" s="81"/>
+      <c r="D15" s="81"/>
       <c r="E15" s="15" t="s">
         <v>2</v>
       </c>
@@ -14850,9 +14850,9 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B16" s="80"/>
-      <c r="C16" s="80"/>
-      <c r="D16" s="80"/>
+      <c r="B16" s="81"/>
+      <c r="C16" s="81"/>
+      <c r="D16" s="81"/>
       <c r="E16" s="11" t="s">
         <v>65</v>
       </c>
@@ -14873,9 +14873,9 @@
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B17" s="81"/>
-      <c r="C17" s="81"/>
-      <c r="D17" s="81"/>
+      <c r="B17" s="82"/>
+      <c r="C17" s="82"/>
+      <c r="D17" s="82"/>
       <c r="E17" s="11" t="s">
         <v>66</v>
       </c>
@@ -14896,13 +14896,13 @@
       </c>
     </row>
     <row r="19" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="79">
+      <c r="B19" s="80">
         <v>3</v>
       </c>
-      <c r="C19" s="79" t="s">
+      <c r="C19" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="79" t="s">
+      <c r="D19" s="80" t="s">
         <v>54</v>
       </c>
       <c r="E19" s="15" t="s">
@@ -14930,9 +14930,9 @@
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B20" s="80"/>
-      <c r="C20" s="80"/>
-      <c r="D20" s="80"/>
+      <c r="B20" s="81"/>
+      <c r="C20" s="81"/>
+      <c r="D20" s="81"/>
       <c r="E20" s="15" t="s">
         <v>1</v>
       </c>
@@ -14958,9 +14958,9 @@
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B21" s="81"/>
-      <c r="C21" s="81"/>
-      <c r="D21" s="81"/>
+      <c r="B21" s="82"/>
+      <c r="C21" s="82"/>
+      <c r="D21" s="82"/>
       <c r="E21" s="15" t="s">
         <v>2</v>
       </c>
@@ -14986,13 +14986,13 @@
       </c>
     </row>
     <row r="23" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="79">
+      <c r="B23" s="80">
         <v>4</v>
       </c>
-      <c r="C23" s="79" t="s">
+      <c r="C23" s="80" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="79" t="s">
+      <c r="D23" s="80" t="s">
         <v>55</v>
       </c>
       <c r="E23" s="15" t="s">
@@ -15020,9 +15020,9 @@
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B24" s="80"/>
-      <c r="C24" s="80"/>
-      <c r="D24" s="80"/>
+      <c r="B24" s="81"/>
+      <c r="C24" s="81"/>
+      <c r="D24" s="81"/>
       <c r="E24" s="15" t="s">
         <v>1</v>
       </c>
@@ -15048,9 +15048,9 @@
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B25" s="80"/>
-      <c r="C25" s="80"/>
-      <c r="D25" s="80"/>
+      <c r="B25" s="81"/>
+      <c r="C25" s="81"/>
+      <c r="D25" s="81"/>
       <c r="E25" s="15" t="s">
         <v>2</v>
       </c>
@@ -15076,9 +15076,9 @@
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B26" s="80"/>
-      <c r="C26" s="80"/>
-      <c r="D26" s="80"/>
+      <c r="B26" s="81"/>
+      <c r="C26" s="81"/>
+      <c r="D26" s="81"/>
       <c r="E26" s="11" t="s">
         <v>67</v>
       </c>
@@ -15099,9 +15099,9 @@
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B27" s="81"/>
-      <c r="C27" s="81"/>
-      <c r="D27" s="81"/>
+      <c r="B27" s="82"/>
+      <c r="C27" s="82"/>
+      <c r="D27" s="82"/>
       <c r="E27" s="11" t="s">
         <v>68</v>
       </c>
@@ -15122,13 +15122,13 @@
       </c>
     </row>
     <row r="29" spans="2:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B29" s="79">
+      <c r="B29" s="80">
         <v>5</v>
       </c>
-      <c r="C29" s="79" t="s">
+      <c r="C29" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="D29" s="79" t="s">
+      <c r="D29" s="80" t="s">
         <v>56</v>
       </c>
       <c r="E29" s="15" t="s">
@@ -15156,9 +15156,9 @@
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B30" s="80"/>
-      <c r="C30" s="80"/>
-      <c r="D30" s="80"/>
+      <c r="B30" s="81"/>
+      <c r="C30" s="81"/>
+      <c r="D30" s="81"/>
       <c r="E30" s="15" t="s">
         <v>1</v>
       </c>
@@ -15184,9 +15184,9 @@
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B31" s="80"/>
-      <c r="C31" s="80"/>
-      <c r="D31" s="80"/>
+      <c r="B31" s="81"/>
+      <c r="C31" s="81"/>
+      <c r="D31" s="81"/>
       <c r="E31" s="15" t="s">
         <v>2</v>
       </c>
@@ -15212,9 +15212,9 @@
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B32" s="80"/>
-      <c r="C32" s="80"/>
-      <c r="D32" s="80"/>
+      <c r="B32" s="81"/>
+      <c r="C32" s="81"/>
+      <c r="D32" s="81"/>
       <c r="E32" s="15" t="s">
         <v>57</v>
       </c>
@@ -15235,9 +15235,9 @@
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B33" s="81"/>
-      <c r="C33" s="81"/>
-      <c r="D33" s="81"/>
+      <c r="B33" s="82"/>
+      <c r="C33" s="82"/>
+      <c r="D33" s="82"/>
       <c r="E33" s="11" t="s">
         <v>64</v>
       </c>
@@ -15258,13 +15258,13 @@
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B35" s="82">
+      <c r="B35" s="79">
         <v>6</v>
       </c>
-      <c r="C35" s="82" t="s">
+      <c r="C35" s="79" t="s">
         <v>62</v>
       </c>
-      <c r="D35" s="82" t="s">
+      <c r="D35" s="79" t="s">
         <v>63</v>
       </c>
       <c r="E35" s="11" t="s">
@@ -15292,9 +15292,9 @@
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B36" s="82"/>
-      <c r="C36" s="82"/>
-      <c r="D36" s="82"/>
+      <c r="B36" s="79"/>
+      <c r="C36" s="79"/>
+      <c r="D36" s="79"/>
       <c r="E36" s="28" t="s">
         <v>1</v>
       </c>
@@ -15320,9 +15320,9 @@
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B37" s="82"/>
-      <c r="C37" s="82"/>
-      <c r="D37" s="82"/>
+      <c r="B37" s="79"/>
+      <c r="C37" s="79"/>
+      <c r="D37" s="79"/>
       <c r="E37" s="28" t="s">
         <v>2</v>
       </c>
@@ -15349,18 +15349,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="B29:B33"/>
-    <mergeCell ref="C29:C33"/>
-    <mergeCell ref="D29:D33"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="D23:D27"/>
     <mergeCell ref="B13:B17"/>
     <mergeCell ref="C13:C17"/>
     <mergeCell ref="D13:D17"/>
@@ -15370,6 +15358,18 @@
     <mergeCell ref="D8:D11"/>
     <mergeCell ref="C4:C6"/>
     <mergeCell ref="C8:C11"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="D23:D27"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="C29:C33"/>
+    <mergeCell ref="D29:D33"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20756,53 +20756,18 @@
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="K173:M173"/>
-    <mergeCell ref="K174:M174"/>
-    <mergeCell ref="K165:M165"/>
-    <mergeCell ref="K169:M169"/>
-    <mergeCell ref="K170:M170"/>
-    <mergeCell ref="K171:M171"/>
-    <mergeCell ref="K172:M172"/>
-    <mergeCell ref="K153:M153"/>
-    <mergeCell ref="K154:M154"/>
-    <mergeCell ref="K155:M155"/>
-    <mergeCell ref="K139:M139"/>
-    <mergeCell ref="K146:M146"/>
-    <mergeCell ref="K150:M150"/>
-    <mergeCell ref="K151:M151"/>
-    <mergeCell ref="K152:M152"/>
-    <mergeCell ref="K134:M134"/>
-    <mergeCell ref="K135:M135"/>
-    <mergeCell ref="K136:M136"/>
-    <mergeCell ref="K137:M137"/>
-    <mergeCell ref="K138:M138"/>
-    <mergeCell ref="K120:M120"/>
-    <mergeCell ref="K121:M121"/>
-    <mergeCell ref="K122:M122"/>
-    <mergeCell ref="K123:M123"/>
-    <mergeCell ref="K130:M130"/>
-    <mergeCell ref="K106:M106"/>
-    <mergeCell ref="K107:M107"/>
-    <mergeCell ref="K114:M114"/>
-    <mergeCell ref="K118:M118"/>
-    <mergeCell ref="K119:M119"/>
-    <mergeCell ref="K98:M98"/>
-    <mergeCell ref="K102:M102"/>
-    <mergeCell ref="K103:M103"/>
-    <mergeCell ref="K104:M104"/>
-    <mergeCell ref="K105:M105"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="K34:M34"/>
-    <mergeCell ref="K50:M50"/>
-    <mergeCell ref="K66:M66"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="K42:M42"/>
-    <mergeCell ref="K43:M43"/>
-    <mergeCell ref="K58:M58"/>
-    <mergeCell ref="K26:M26"/>
-    <mergeCell ref="K27:M27"/>
+    <mergeCell ref="K88:M88"/>
+    <mergeCell ref="K89:M89"/>
+    <mergeCell ref="K90:M90"/>
+    <mergeCell ref="K56:M56"/>
+    <mergeCell ref="K57:M57"/>
+    <mergeCell ref="K59:M59"/>
+    <mergeCell ref="K86:M86"/>
+    <mergeCell ref="K87:M87"/>
+    <mergeCell ref="K71:M71"/>
+    <mergeCell ref="K72:M72"/>
+    <mergeCell ref="K73:M73"/>
+    <mergeCell ref="K70:M70"/>
     <mergeCell ref="K91:M91"/>
     <mergeCell ref="K10:M10"/>
     <mergeCell ref="K11:M11"/>
@@ -20819,18 +20784,53 @@
     <mergeCell ref="K82:M82"/>
     <mergeCell ref="K74:M74"/>
     <mergeCell ref="K75:M75"/>
-    <mergeCell ref="K88:M88"/>
-    <mergeCell ref="K89:M89"/>
-    <mergeCell ref="K90:M90"/>
-    <mergeCell ref="K56:M56"/>
-    <mergeCell ref="K57:M57"/>
-    <mergeCell ref="K59:M59"/>
-    <mergeCell ref="K86:M86"/>
-    <mergeCell ref="K87:M87"/>
-    <mergeCell ref="K71:M71"/>
-    <mergeCell ref="K72:M72"/>
-    <mergeCell ref="K73:M73"/>
-    <mergeCell ref="K70:M70"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="K50:M50"/>
+    <mergeCell ref="K66:M66"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="K42:M42"/>
+    <mergeCell ref="K43:M43"/>
+    <mergeCell ref="K58:M58"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="K27:M27"/>
+    <mergeCell ref="K98:M98"/>
+    <mergeCell ref="K102:M102"/>
+    <mergeCell ref="K103:M103"/>
+    <mergeCell ref="K104:M104"/>
+    <mergeCell ref="K105:M105"/>
+    <mergeCell ref="K106:M106"/>
+    <mergeCell ref="K107:M107"/>
+    <mergeCell ref="K114:M114"/>
+    <mergeCell ref="K118:M118"/>
+    <mergeCell ref="K119:M119"/>
+    <mergeCell ref="K120:M120"/>
+    <mergeCell ref="K121:M121"/>
+    <mergeCell ref="K122:M122"/>
+    <mergeCell ref="K123:M123"/>
+    <mergeCell ref="K130:M130"/>
+    <mergeCell ref="K134:M134"/>
+    <mergeCell ref="K135:M135"/>
+    <mergeCell ref="K136:M136"/>
+    <mergeCell ref="K137:M137"/>
+    <mergeCell ref="K138:M138"/>
+    <mergeCell ref="K153:M153"/>
+    <mergeCell ref="K154:M154"/>
+    <mergeCell ref="K155:M155"/>
+    <mergeCell ref="K139:M139"/>
+    <mergeCell ref="K146:M146"/>
+    <mergeCell ref="K150:M150"/>
+    <mergeCell ref="K151:M151"/>
+    <mergeCell ref="K152:M152"/>
+    <mergeCell ref="K173:M173"/>
+    <mergeCell ref="K174:M174"/>
+    <mergeCell ref="K165:M165"/>
+    <mergeCell ref="K169:M169"/>
+    <mergeCell ref="K170:M170"/>
+    <mergeCell ref="K171:M171"/>
+    <mergeCell ref="K172:M172"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20843,7 +20843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
@@ -22534,28 +22534,28 @@
       </c>
       <c r="D31" s="74">
         <f>塔_属性!C31</f>
-        <v>88.23</v>
+        <v>48.23</v>
       </c>
       <c r="E31" s="29" t="s">
         <v>70</v>
       </c>
       <c r="F31" s="74">
         <f>塔_属性!D31</f>
-        <v>210.08</v>
+        <v>160.08000000000001</v>
       </c>
       <c r="G31" s="29" t="s">
         <v>70</v>
       </c>
       <c r="H31" s="29">
         <f>塔_属性!E31</f>
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I31" s="29" t="s">
         <v>70</v>
       </c>
       <c r="J31" s="29">
         <f>塔_属性!F31</f>
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="K31" s="29" t="s">
         <v>70</v>

</xml_diff>